<commit_message>
Added try-catch in SQLHandler.
</commit_message>
<xml_diff>
--- a/files/123.xlsx
+++ b/files/123.xlsx
@@ -14,27 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31252" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="7">
   <si>
-    <t>Alex|Krylov</t>
+    <t>slate@list.ru</t>
   </si>
   <si>
-    <t>Petrov|Vladimir</t>
+    <t>vlad@list.ru</t>
   </si>
   <si>
-    <t>Popov|Sergei</t>
+    <t>ser@list.ru</t>
   </si>
   <si>
-    <t>Ivanov|Albert</t>
+    <t>albiv@list.ru</t>
   </si>
   <si>
-    <t>Serov|Valera</t>
+    <t>vals@list.ru</t>
   </si>
   <si>
-    <t>Ponov|Pavel</t>
+    <t>popov@list.ru</t>
   </si>
   <si>
-    <t>Okolov|Seva</t>
+    <t>seva@list.ru</t>
   </si>
 </sst>
 </file>
@@ -380,13 +380,10 @@
   <dimension ref="A1:C840"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A694" workbookViewId="0">
-      <selection activeCell="A721" sqref="A721:A840"/>
+      <selection activeCell="B694" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" customWidth="true" width="28.28515625" collapsed="true"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">

</xml_diff>